<commit_message>
Leakage test / Jankowski comparison samples
Worked through processing the leakage test data (not quite done yet);
finished processing the Nov 2014 flux info for comparison between
O’Connell and Jankowski protocols
</commit_message>
<xml_diff>
--- a/GC-Data-Raw-R/GC-Data-standardizedfilenames/runsheets-standardizedfilenames/runsheet_20140606_Leak0.xlsx
+++ b/GC-Data-Raw-R/GC-Data-standardizedfilenames/runsheets-standardizedfilenames/runsheet_20140606_Leak0.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="13900" yWindow="5260" windowWidth="18920" windowHeight="13220" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="26">
   <si>
     <t>SampleName</t>
   </si>
@@ -82,6 +82,21 @@
   </si>
   <si>
     <t>2014.06.06</t>
+  </si>
+  <si>
+    <t>Mix1Leak</t>
+  </si>
+  <si>
+    <t>Mix2Leak</t>
+  </si>
+  <si>
+    <t>3N2OLeak</t>
+  </si>
+  <si>
+    <t>10N2OLeak</t>
+  </si>
+  <si>
+    <t>3KCO2Leak</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1079,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1120,7 +1135,7 @@
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
@@ -1152,7 +1167,7 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
@@ -1184,7 +1199,7 @@
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
         <v>16</v>
@@ -1216,7 +1231,7 @@
         <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
@@ -1248,7 +1263,7 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
         <v>16</v>
@@ -1280,7 +1295,7 @@
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
@@ -1312,7 +1327,7 @@
         <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
@@ -1344,7 +1359,7 @@
         <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
@@ -1376,7 +1391,7 @@
         <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F10" t="s">
         <v>16</v>
@@ -1408,7 +1423,7 @@
         <v>19</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F11" t="s">
         <v>16</v>
@@ -1440,7 +1455,7 @@
         <v>19</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
@@ -1472,7 +1487,7 @@
         <v>19</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
@@ -1504,7 +1519,7 @@
         <v>19</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F14" t="s">
         <v>16</v>
@@ -1536,7 +1551,7 @@
         <v>19</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
         <v>16</v>
@@ -1568,7 +1583,7 @@
         <v>19</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F16" t="s">
         <v>16</v>

</xml_diff>